<commit_message>
Added more test to smoke data set
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Hasanein.Ba-Alawi.AuthorisedRep</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -484,9 +481,6 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -495,9 +489,6 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -506,9 +497,6 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -517,9 +505,6 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -528,9 +513,6 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -538,9 +520,6 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a new check to make sure page is loaded before we do anything
WaitUtils.isPageLoadingComplete(driver, TIMEOUT_PAGE_LOAD);
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/data/excel/users.xlsx
+++ b/src/test/resources/configs/data/excel/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Hasanein.Ba-Alawi.AuthorisedRep</t>
+  </si>
+  <si>
+    <t>MHRA12345</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +458,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>